<commit_message>
changes to all files
</commit_message>
<xml_diff>
--- a/files/04_Testbericht.xlsx
+++ b/files/04_Testbericht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\M242\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B8A12D4-88C4-4FCC-884A-76C4AA0EBDD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC85F0F0-4074-4CF4-BF59-C52888B5FE43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{237AC24E-75B3-43AA-8007-EFE1360D46CB}"/>
   </bookViews>
@@ -33,25 +33,95 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>Testfälle M242</t>
+  </si>
+  <si>
+    <t>Erwartet</t>
+  </si>
+  <si>
+    <t>Effektiv</t>
+  </si>
+  <si>
+    <t>Massnahmen</t>
+  </si>
+  <si>
+    <t>Ein Licht füllt die Reihe Lampe für Lampe auf.</t>
+  </si>
+  <si>
+    <t>Trifft zu</t>
+  </si>
+  <si>
+    <t>Mit einem Knopf kann das Lauflicht gestoppt, respektive gestartet werden.</t>
+  </si>
+  <si>
+    <t>Das Lauflicht läuft in einem Sekundentakt.</t>
+  </si>
+  <si>
+    <t>Während dem Stop werden alle LED's deaktiviert.</t>
+  </si>
+  <si>
+    <t>Die Geschwindigkeit ist verstellbar.</t>
+  </si>
+  <si>
+    <t>Die Laufwechslung kann während dem Stopp gewechselt werden.</t>
+  </si>
+  <si>
+    <t>Die Laufwechslung kann während der Pause gewechselt werden.</t>
+  </si>
+  <si>
+    <t>Die Breite des Effektes kann verstellt werden.</t>
+  </si>
+  <si>
+    <t>Beim Start kommt ein Intro-Lichtspiel</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -59,17 +129,426 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -80,6 +559,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14C7E34C-A579-4FB0-8B55-66AB3816C44D}" name="Table1" displayName="Table1" ref="B4:F13" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6">
+  <autoFilter ref="B4:F13" xr:uid="{598CBE8E-2B89-45E6-8A3F-FA00C9CF9CAE}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{752488E4-C203-4996-BBB3-688702F90B1F}" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{631303E4-C035-4E15-9D14-839E0D01FF88}" name="Beschreibung"/>
+    <tableColumn id="3" xr3:uid="{C779A686-5547-4193-9544-B9D8B7D2B021}" name="Erwartet" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{4881E8F2-9763-445F-8963-61C82F2F05E5}" name="Effektiv" dataDxfId="2" dataCellStyle="Good"/>
+    <tableColumn id="5" xr3:uid="{7252AD56-C3F1-4C5F-9052-3249AACE9348}" name="Massnahmen" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,12 +872,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2E6A92-96F9-4B7B-A552-2C28C4AF8379}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="67.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="15">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="15">
+        <v>2</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="15">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="16">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="14">
+        <v>5</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="17">
+        <v>6</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="15">
+        <v>7</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="15">
+        <v>8</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="16">
+        <v>9</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>